<commit_message>
updates to db and xlsx files
</commit_message>
<xml_diff>
--- a/Tables&Relations.xlsx
+++ b/Tables&Relations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgrifit\Desktop\IIT\OnlineTraining\Spring2018\OpenSourceProgramming\FinalProject_DueApr29\ghrepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1454DB82-AA39-463A-B36C-E213CDB77E7D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EA2578-30E1-4717-81A4-F90478949946}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20355" windowHeight="10830" xr2:uid="{F62A5D56-28AC-4B05-9321-33328E52EE30}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20355" windowHeight="10830" firstSheet="1" activeTab="2" xr2:uid="{F62A5D56-28AC-4B05-9321-33328E52EE30}"/>
   </bookViews>
   <sheets>
     <sheet name="Table Relations" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="175">
   <si>
     <t>fname</t>
   </si>
@@ -539,9 +539,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>Reference Is Available - is_available_val</t>
-  </si>
-  <si>
     <t>Reference Patient - patient_id</t>
   </si>
   <si>
@@ -554,7 +551,7 @@
     <t>Reference Procedure - procedure_id</t>
   </si>
   <si>
-    <t>is_available_val_pid</t>
+    <t>Reference Is Available - is_available_pid</t>
   </si>
 </sst>
 </file>
@@ -595,7 +592,7 @@
       <patternFill patternType="darkGrid"/>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -952,19 +949,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1081,7 +1065,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1136,7 +1120,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1163,10 +1146,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1231,51 +1214,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1288,13 +1226,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1302,6 +1249,42 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -7372,8 +7355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D224C6BA-3041-4FF2-9ED2-49CADB590F58}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="B45" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7386,31 +7369,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="77"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="79"/>
       <c r="E1" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="82">
+      <c r="A2" s="66">
         <v>1</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="75"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="82"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="82"/>
+      <c r="A3" s="66"/>
       <c r="B3" s="4" t="s">
         <v>117</v>
       </c>
@@ -7423,7 +7406,7 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="82"/>
+      <c r="A4" s="66"/>
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
@@ -7436,7 +7419,7 @@
       <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="82"/>
+      <c r="A5" s="66"/>
       <c r="B5" s="10" t="s">
         <v>1</v>
       </c>
@@ -7449,18 +7432,18 @@
       <c r="E5" s="15"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="89">
+      <c r="A6" s="76">
         <v>2</v>
       </c>
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="75"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="82"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="82"/>
+      <c r="A7" s="66"/>
       <c r="B7" s="4" t="s">
         <v>118</v>
       </c>
@@ -7473,7 +7456,7 @@
       <c r="E7" s="17"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="82"/>
+      <c r="A8" s="66"/>
       <c r="B8" s="7" t="s">
         <v>0</v>
       </c>
@@ -7486,7 +7469,7 @@
       <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="90"/>
+      <c r="A9" s="77"/>
       <c r="B9" s="18" t="s">
         <v>0</v>
       </c>
@@ -7499,18 +7482,18 @@
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="89">
+      <c r="A10" s="76">
         <v>3</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="75"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="82"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="82"/>
+      <c r="A11" s="66"/>
       <c r="B11" s="4" t="s">
         <v>120</v>
       </c>
@@ -7523,7 +7506,7 @@
       <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="82"/>
+      <c r="A12" s="66"/>
       <c r="B12" s="7" t="s">
         <v>0</v>
       </c>
@@ -7536,7 +7519,7 @@
       <c r="E12" s="14"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="90"/>
+      <c r="A13" s="77"/>
       <c r="B13" s="18" t="s">
         <v>1</v>
       </c>
@@ -7549,18 +7532,18 @@
       <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="89">
+      <c r="A14" s="76">
         <v>4</v>
       </c>
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="75"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="82"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="82"/>
+      <c r="A15" s="66"/>
       <c r="B15" s="4" t="s">
         <v>121</v>
       </c>
@@ -7573,7 +7556,7 @@
       <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="90"/>
+      <c r="A16" s="77"/>
       <c r="B16" s="18" t="s">
         <v>27</v>
       </c>
@@ -7586,18 +7569,18 @@
       <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="89">
+      <c r="A17" s="76">
         <v>5</v>
       </c>
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="75"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="82"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="82"/>
+      <c r="A18" s="66"/>
       <c r="B18" s="4" t="s">
         <v>122</v>
       </c>
@@ -7610,7 +7593,7 @@
       <c r="E18" s="17"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="90"/>
+      <c r="A19" s="77"/>
       <c r="B19" s="18" t="s">
         <v>21</v>
       </c>
@@ -7623,176 +7606,176 @@
       <c r="E19" s="16"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="86">
+      <c r="A20" s="73">
         <v>6</v>
       </c>
-      <c r="B20" s="81" t="s">
+      <c r="B20" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="69"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="88"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="87"/>
+      <c r="A21" s="74"/>
       <c r="B21" s="4" t="s">
         <v>123</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="34"/>
+      <c r="E21" s="33"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="87"/>
+      <c r="A22" s="74"/>
       <c r="B22" s="7" t="s">
         <v>112</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="28">
+      <c r="D22" s="27">
         <v>26</v>
       </c>
-      <c r="E22" s="29"/>
+      <c r="E22" s="28"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="88"/>
+      <c r="A23" s="75"/>
       <c r="B23" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="36">
+      <c r="D23" s="35">
         <v>26</v>
       </c>
-      <c r="E23" s="37"/>
+      <c r="E23" s="36"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="89">
+      <c r="A24" s="76">
         <v>7</v>
       </c>
-      <c r="B24" s="81" t="s">
+      <c r="B24" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="69"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="88"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="82"/>
+      <c r="A25" s="66"/>
       <c r="B25" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="34"/>
+      <c r="E25" s="33"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="90"/>
+      <c r="A26" s="77"/>
       <c r="B26" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="C26" s="35" t="s">
+      <c r="C26" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="36">
+      <c r="D26" s="35">
         <v>8</v>
       </c>
-      <c r="E26" s="37"/>
+      <c r="E26" s="36"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="89">
+      <c r="A27" s="76">
         <v>8</v>
       </c>
-      <c r="B27" s="67" t="s">
+      <c r="B27" s="89" t="s">
         <v>115</v>
       </c>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="69"/>
+      <c r="C27" s="87"/>
+      <c r="D27" s="87"/>
+      <c r="E27" s="88"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="82"/>
-      <c r="B28" s="39" t="s">
+      <c r="A28" s="66"/>
+      <c r="B28" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="C28" s="38" t="s">
+      <c r="C28" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="34"/>
+      <c r="E28" s="33"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="90"/>
-      <c r="B29" s="40" t="s">
+      <c r="A29" s="77"/>
+      <c r="B29" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="31">
+      <c r="D29" s="30">
         <v>8</v>
       </c>
-      <c r="E29" s="32"/>
+      <c r="E29" s="31"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="89">
+      <c r="A30" s="76">
         <v>9</v>
       </c>
-      <c r="B30" s="67" t="s">
+      <c r="B30" s="89" t="s">
         <v>142</v>
       </c>
-      <c r="C30" s="68"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="69"/>
+      <c r="C30" s="87"/>
+      <c r="D30" s="87"/>
+      <c r="E30" s="88"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="82"/>
-      <c r="B31" s="39" t="s">
+      <c r="A31" s="66"/>
+      <c r="B31" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="C31" s="38" t="s">
+      <c r="C31" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="34"/>
+      <c r="E31" s="33"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="90"/>
-      <c r="B32" s="40" t="s">
+      <c r="A32" s="77"/>
+      <c r="B32" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="31">
+      <c r="D32" s="30">
         <v>8</v>
       </c>
-      <c r="E32" s="32"/>
+      <c r="E32" s="31"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="70">
         <v>10</v>
       </c>
-      <c r="B33" s="73" t="s">
+      <c r="B33" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="74"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="75"/>
+      <c r="C33" s="81"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="82"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="71"/>
@@ -7864,19 +7847,19 @@
         <v>4</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="70">
         <v>11</v>
       </c>
-      <c r="B39" s="73" t="s">
+      <c r="B39" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="74"/>
-      <c r="D39" s="74"/>
-      <c r="E39" s="75"/>
+      <c r="C39" s="81"/>
+      <c r="D39" s="81"/>
+      <c r="E39" s="82"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="71"/>
@@ -7939,26 +7922,28 @@
     <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="72"/>
       <c r="B44" s="18" t="s">
-        <v>175</v>
+        <v>143</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="12">
-        <v>1</v>
-      </c>
-      <c r="E44" s="24"/>
+      <c r="D44" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="23" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="70">
         <v>12</v>
       </c>
-      <c r="B45" s="73" t="s">
+      <c r="B45" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="74"/>
-      <c r="D45" s="74"/>
-      <c r="E45" s="75"/>
+      <c r="C45" s="81"/>
+      <c r="D45" s="81"/>
+      <c r="E45" s="82"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="71"/>
@@ -7985,7 +7970,7 @@
         <v>4</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -8000,7 +7985,7 @@
         <v>4</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -8015,7 +8000,7 @@
         <v>4</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -8030,7 +8015,7 @@
         <v>4</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -8093,12 +8078,12 @@
       <c r="A55" s="70">
         <v>13</v>
       </c>
-      <c r="B55" s="73" t="s">
+      <c r="B55" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="74"/>
-      <c r="D55" s="74"/>
-      <c r="E55" s="75"/>
+      <c r="C55" s="81"/>
+      <c r="D55" s="81"/>
+      <c r="E55" s="82"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="71"/>
@@ -8156,161 +8141,149 @@
     </row>
     <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="83"/>
-      <c r="B61" s="78" t="s">
+      <c r="A61" s="67"/>
+      <c r="B61" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="C61" s="79"/>
-      <c r="D61" s="79"/>
-      <c r="E61" s="80"/>
+      <c r="C61" s="84"/>
+      <c r="D61" s="84"/>
+      <c r="E61" s="85"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="84"/>
-      <c r="B62" s="50" t="s">
+      <c r="A62" s="68"/>
+      <c r="B62" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="C62" s="51" t="s">
+      <c r="C62" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="D62" s="52" t="s">
+      <c r="D62" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E62" s="53"/>
+      <c r="E62" s="52"/>
     </row>
     <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="85"/>
-      <c r="B63" s="54" t="s">
+      <c r="A63" s="69"/>
+      <c r="B63" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="C63" s="55" t="s">
+      <c r="C63" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D63" s="56">
+      <c r="D63" s="55">
         <v>45</v>
       </c>
-      <c r="E63" s="57"/>
+      <c r="E63" s="56"/>
     </row>
     <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="83"/>
-      <c r="B65" s="78" t="s">
+      <c r="A65" s="67"/>
+      <c r="B65" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="C65" s="79"/>
-      <c r="D65" s="79"/>
-      <c r="E65" s="80"/>
+      <c r="C65" s="84"/>
+      <c r="D65" s="84"/>
+      <c r="E65" s="85"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="84"/>
-      <c r="B66" s="50" t="s">
+      <c r="A66" s="68"/>
+      <c r="B66" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="C66" s="51" t="s">
+      <c r="C66" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="D66" s="52" t="s">
+      <c r="D66" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E66" s="58"/>
+      <c r="E66" s="57"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="84"/>
-      <c r="B67" s="59" t="s">
+      <c r="A67" s="68"/>
+      <c r="B67" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="C67" s="60" t="s">
+      <c r="C67" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="D67" s="61" t="s">
+      <c r="D67" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="E67" s="62" t="s">
+      <c r="E67" s="61" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="85"/>
-      <c r="B68" s="54" t="s">
+      <c r="A68" s="69"/>
+      <c r="B68" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="C68" s="55" t="s">
+      <c r="C68" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="D68" s="56" t="s">
+      <c r="D68" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E68" s="63" t="s">
+      <c r="E68" s="62" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="83"/>
-      <c r="B70" s="78" t="s">
+      <c r="A70" s="67"/>
+      <c r="B70" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="C70" s="79"/>
-      <c r="D70" s="79"/>
-      <c r="E70" s="80"/>
+      <c r="C70" s="84"/>
+      <c r="D70" s="84"/>
+      <c r="E70" s="85"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="84"/>
-      <c r="B71" s="50" t="s">
+      <c r="A71" s="68"/>
+      <c r="B71" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="C71" s="51" t="s">
+      <c r="C71" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="D71" s="52" t="s">
+      <c r="D71" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E71" s="58"/>
+      <c r="E71" s="57"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="84"/>
-      <c r="B72" s="59" t="s">
+      <c r="A72" s="68"/>
+      <c r="B72" s="58" t="s">
         <v>118</v>
       </c>
-      <c r="C72" s="60" t="s">
+      <c r="C72" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="D72" s="61" t="s">
+      <c r="D72" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="E72" s="62" t="s">
+      <c r="E72" s="61" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="85"/>
-      <c r="B73" s="54" t="s">
+      <c r="A73" s="69"/>
+      <c r="B73" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="C73" s="55" t="s">
+      <c r="C73" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="D73" s="56" t="s">
+      <c r="D73" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="E73" s="63" t="s">
+      <c r="E73" s="62" t="s">
         <v>134</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="A55:A59"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B33:E33"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B6:E6"/>
@@ -8326,11 +8299,23 @@
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="A55:A59"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A30:A32"/>
     <mergeCell ref="A45:A54"/>
     <mergeCell ref="A39:A44"/>
-    <mergeCell ref="B39:E39"/>
     <mergeCell ref="A33:A38"/>
-    <mergeCell ref="B33:E33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8357,19 +8342,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="G1" s="91" t="s">
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="G1" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="91"/>
-      <c r="L1" s="91" t="s">
+      <c r="H1" s="90"/>
+      <c r="L1" s="90" t="s">
         <v>150</v>
       </c>
-      <c r="M1" s="91"/>
+      <c r="M1" s="90"/>
       <c r="S1" s="2" t="s">
         <v>23</v>
       </c>
@@ -8629,19 +8614,19 @@
     </row>
     <row r="12" spans="1:20" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="91" t="s">
+      <c r="A13" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="91"/>
-      <c r="C13" s="91"/>
-      <c r="G13" s="91" t="s">
+      <c r="B13" s="90"/>
+      <c r="C13" s="90"/>
+      <c r="G13" s="90" t="s">
         <v>102</v>
       </c>
-      <c r="H13" s="91"/>
-      <c r="L13" s="91" t="s">
+      <c r="H13" s="90"/>
+      <c r="L13" s="90" t="s">
         <v>142</v>
       </c>
-      <c r="M13" s="91"/>
+      <c r="M13" s="90"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -8742,15 +8727,15 @@
     </row>
     <row r="19" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="91" t="s">
+      <c r="A20" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="91"/>
-      <c r="C20" s="91"/>
-      <c r="G20" s="91" t="s">
+      <c r="B20" s="90"/>
+      <c r="C20" s="90"/>
+      <c r="G20" s="90" t="s">
         <v>157</v>
       </c>
-      <c r="H20" s="91"/>
+      <c r="H20" s="90"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -9034,8 +9019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99330B9-CAFA-4822-8F10-146FD06622F1}">
   <dimension ref="B1:AJ36"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="V39" sqref="V38:V39"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9070,37 +9055,37 @@
   <sheetData>
     <row r="1" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="75"/>
-      <c r="F2" s="73" t="s">
+      <c r="C2" s="81"/>
+      <c r="D2" s="82"/>
+      <c r="F2" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="74"/>
-      <c r="H2" s="75"/>
-      <c r="J2" s="73" t="s">
+      <c r="G2" s="81"/>
+      <c r="H2" s="82"/>
+      <c r="J2" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="74"/>
-      <c r="L2" s="75"/>
-      <c r="N2" s="73" t="s">
+      <c r="K2" s="81"/>
+      <c r="L2" s="82"/>
+      <c r="N2" s="80" t="s">
         <v>141</v>
       </c>
-      <c r="O2" s="74"/>
-      <c r="P2" s="75"/>
-      <c r="R2" s="81" t="s">
+      <c r="O2" s="81"/>
+      <c r="P2" s="82"/>
+      <c r="R2" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="S2" s="68"/>
-      <c r="T2" s="69"/>
-      <c r="V2" s="81" t="s">
+      <c r="S2" s="87"/>
+      <c r="T2" s="88"/>
+      <c r="V2" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="W2" s="68"/>
-      <c r="X2" s="69"/>
-      <c r="AG2" s="46"/>
+      <c r="W2" s="87"/>
+      <c r="X2" s="88"/>
+      <c r="AG2" s="45"/>
     </row>
     <row r="3" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -9142,10 +9127,10 @@
       <c r="R3" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="S3" s="38" t="s">
+      <c r="S3" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="T3" s="43" t="s">
+      <c r="T3" s="42" t="s">
         <v>3</v>
       </c>
       <c r="V3" s="4" t="s">
@@ -9154,10 +9139,10 @@
       <c r="W3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="X3" s="43" t="s">
+      <c r="X3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="AG3" s="26"/>
+      <c r="AG3" s="25"/>
     </row>
     <row r="4" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
@@ -9199,10 +9184,10 @@
       <c r="R4" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="S4" s="30" t="s">
+      <c r="S4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="T4" s="45">
+      <c r="T4" s="44">
         <v>8</v>
       </c>
       <c r="V4" s="7" t="s">
@@ -9211,10 +9196,10 @@
       <c r="W4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="X4" s="44">
+      <c r="X4" s="43">
         <v>26</v>
       </c>
-      <c r="AG4" s="26"/>
+      <c r="AG4" s="25"/>
     </row>
     <row r="5" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
@@ -9247,68 +9232,68 @@
       <c r="V5" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="W5" s="30" t="s">
+      <c r="W5" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="X5" s="45">
+      <c r="X5" s="44">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="42"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="42"/>
-      <c r="AH6" s="41"/>
-      <c r="AI6" s="26"/>
-      <c r="AJ6" s="27"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="41"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="41"/>
+      <c r="AH6" s="40"/>
+      <c r="AI6" s="25"/>
+      <c r="AJ6" s="26"/>
     </row>
     <row r="7" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="42"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="42"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="42"/>
-      <c r="AH7" s="41"/>
-      <c r="AI7" s="26"/>
-      <c r="AJ7" s="27"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="41"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="41"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="41"/>
+      <c r="AH7" s="40"/>
+      <c r="AI7" s="25"/>
+      <c r="AJ7" s="26"/>
     </row>
     <row r="9" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="74"/>
-      <c r="D10" s="75"/>
-      <c r="F10" s="73" t="s">
+      <c r="C10" s="81"/>
+      <c r="D10" s="82"/>
+      <c r="F10" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="74"/>
-      <c r="H10" s="75"/>
-      <c r="J10" s="73" t="s">
+      <c r="G10" s="81"/>
+      <c r="H10" s="82"/>
+      <c r="J10" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="74"/>
-      <c r="L10" s="75"/>
-      <c r="N10" s="73" t="s">
+      <c r="K10" s="81"/>
+      <c r="L10" s="82"/>
+      <c r="N10" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="O10" s="74"/>
-      <c r="P10" s="75"/>
-      <c r="R10" s="81" t="s">
+      <c r="O10" s="81"/>
+      <c r="P10" s="82"/>
+      <c r="R10" s="86" t="s">
         <v>115</v>
       </c>
-      <c r="S10" s="68"/>
-      <c r="T10" s="69"/>
+      <c r="S10" s="87"/>
+      <c r="T10" s="88"/>
     </row>
     <row r="11" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
@@ -9350,10 +9335,10 @@
       <c r="R11" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="S11" s="38" t="s">
+      <c r="S11" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="T11" s="43" t="s">
+      <c r="T11" s="42" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9397,10 +9382,10 @@
       <c r="R12" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="S12" s="30" t="s">
+      <c r="S12" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="T12" s="45">
+      <c r="T12" s="44">
         <v>8</v>
       </c>
     </row>
@@ -9424,7 +9409,7 @@
         <v>29</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>7</v>
@@ -9462,7 +9447,7 @@
         <v>29</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="K14" s="8" t="s">
         <v>7</v>
@@ -9519,11 +9504,11 @@
       </c>
     </row>
     <row r="17" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="92" t="s">
+      <c r="B17" s="91" t="s">
         <v>142</v>
       </c>
-      <c r="C17" s="93"/>
-      <c r="D17" s="94"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="93"/>
       <c r="J17" s="7" t="s">
         <v>136</v>
       </c>
@@ -9535,13 +9520,13 @@
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="47" t="s">
         <v>143</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="43" t="s">
+      <c r="D18" s="42" t="s">
         <v>3</v>
       </c>
       <c r="J18" s="7" t="s">
@@ -9555,13 +9540,13 @@
       </c>
     </row>
     <row r="19" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="45">
+      <c r="D19" s="44">
         <v>6</v>
       </c>
       <c r="J19" s="10" t="s">
@@ -9573,14 +9558,14 @@
       <c r="L19" s="12"/>
     </row>
     <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="N20" s="73" t="s">
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="N20" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="O20" s="74"/>
-      <c r="P20" s="75"/>
+      <c r="O20" s="81"/>
+      <c r="P20" s="82"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N21" s="4" t="s">
@@ -9606,102 +9591,109 @@
     </row>
     <row r="32" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="78" t="s">
+      <c r="B33" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="79"/>
-      <c r="D33" s="80"/>
-      <c r="F33" s="78" t="s">
+      <c r="C33" s="84"/>
+      <c r="D33" s="85"/>
+      <c r="F33" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="G33" s="79"/>
-      <c r="H33" s="80"/>
-      <c r="J33" s="78" t="s">
+      <c r="G33" s="84"/>
+      <c r="H33" s="85"/>
+      <c r="J33" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="K33" s="79"/>
-      <c r="L33" s="80"/>
+      <c r="K33" s="84"/>
+      <c r="L33" s="85"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="C34" s="51" t="s">
+      <c r="C34" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="52" t="s">
+      <c r="D34" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="50" t="s">
+      <c r="F34" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="G34" s="51" t="s">
+      <c r="G34" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="H34" s="52" t="s">
+      <c r="H34" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="J34" s="50" t="s">
+      <c r="J34" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="K34" s="51" t="s">
+      <c r="K34" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="L34" s="52" t="s">
+      <c r="L34" s="51" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="35" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="59" t="s">
+      <c r="B35" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="C35" s="60" t="s">
+      <c r="C35" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="61" t="s">
+      <c r="D35" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="F35" s="59" t="s">
+      <c r="F35" s="58" t="s">
         <v>118</v>
       </c>
-      <c r="G35" s="60" t="s">
+      <c r="G35" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="H35" s="61" t="s">
+      <c r="H35" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="J35" s="64" t="s">
+      <c r="J35" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="K35" s="65" t="s">
+      <c r="K35" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="L35" s="66">
+      <c r="L35" s="65">
         <v>45</v>
       </c>
     </row>
     <row r="36" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="64" t="s">
+      <c r="B36" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="C36" s="65" t="s">
+      <c r="C36" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="66" t="s">
+      <c r="D36" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F36" s="64" t="s">
+      <c r="F36" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="G36" s="65" t="s">
+      <c r="G36" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="H36" s="66" t="s">
+      <c r="H36" s="65" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="J2:L2"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="F33:H33"/>
     <mergeCell ref="N10:P10"/>
@@ -9711,13 +9703,6 @@
     <mergeCell ref="N20:P20"/>
     <mergeCell ref="J33:L33"/>
     <mergeCell ref="B17:D17"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="J2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated sql and xlsx files
</commit_message>
<xml_diff>
--- a/Tables&Relations.xlsx
+++ b/Tables&Relations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgrifit\Desktop\IIT\OnlineTraining\Spring2018\OpenSourceProgramming\FinalProject_DueApr29\ghrepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EA2578-30E1-4717-81A4-F90478949946}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E4C01D-6FC7-4026-AF2B-CD5021068236}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20355" windowHeight="10830" firstSheet="1" activeTab="2" xr2:uid="{F62A5D56-28AC-4B05-9321-33328E52EE30}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20355" windowHeight="10830" xr2:uid="{F62A5D56-28AC-4B05-9321-33328E52EE30}"/>
   </bookViews>
   <sheets>
     <sheet name="Table Relations" sheetId="2" r:id="rId1"/>
@@ -542,16 +542,16 @@
     <t>Reference Patient - patient_id</t>
   </si>
   <si>
-    <t>Reference Nurse Availability - nurse_availability_id</t>
-  </si>
-  <si>
-    <t>Reference Doctor Availability - doctor_availability_id</t>
-  </si>
-  <si>
     <t>Reference Procedure - procedure_id</t>
   </si>
   <si>
     <t>Reference Is Available - is_available_pid</t>
+  </si>
+  <si>
+    <t>Reference Doctor Availability - doctor_id</t>
+  </si>
+  <si>
+    <t>Reference Nurse Availability - nurse_id</t>
   </si>
 </sst>
 </file>
@@ -1214,6 +1214,42 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1249,42 +1285,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -7355,8 +7355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D224C6BA-3041-4FF2-9ED2-49CADB590F58}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="B45" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7372,28 +7372,28 @@
       <c r="A1" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="79"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="70"/>
       <c r="E1" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="66">
+      <c r="A2" s="78">
         <v>1</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="82"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="68"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="66"/>
+      <c r="A3" s="78"/>
       <c r="B3" s="4" t="s">
         <v>117</v>
       </c>
@@ -7406,7 +7406,7 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="66"/>
+      <c r="A4" s="78"/>
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
@@ -7419,7 +7419,7 @@
       <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="66"/>
+      <c r="A5" s="78"/>
       <c r="B5" s="10" t="s">
         <v>1</v>
       </c>
@@ -7432,18 +7432,18 @@
       <c r="E5" s="15"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="76">
+      <c r="A6" s="88">
         <v>2</v>
       </c>
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="82"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="68"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="66"/>
+      <c r="A7" s="78"/>
       <c r="B7" s="4" t="s">
         <v>118</v>
       </c>
@@ -7456,7 +7456,7 @@
       <c r="E7" s="17"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="66"/>
+      <c r="A8" s="78"/>
       <c r="B8" s="7" t="s">
         <v>0</v>
       </c>
@@ -7469,7 +7469,7 @@
       <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="77"/>
+      <c r="A9" s="89"/>
       <c r="B9" s="18" t="s">
         <v>0</v>
       </c>
@@ -7482,18 +7482,18 @@
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="76">
+      <c r="A10" s="88">
         <v>3</v>
       </c>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="82"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="68"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
+      <c r="A11" s="78"/>
       <c r="B11" s="4" t="s">
         <v>120</v>
       </c>
@@ -7506,7 +7506,7 @@
       <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="66"/>
+      <c r="A12" s="78"/>
       <c r="B12" s="7" t="s">
         <v>0</v>
       </c>
@@ -7519,7 +7519,7 @@
       <c r="E12" s="14"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="77"/>
+      <c r="A13" s="89"/>
       <c r="B13" s="18" t="s">
         <v>1</v>
       </c>
@@ -7532,18 +7532,18 @@
       <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="76">
+      <c r="A14" s="88">
         <v>4</v>
       </c>
-      <c r="B14" s="80" t="s">
+      <c r="B14" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="81"/>
-      <c r="D14" s="81"/>
-      <c r="E14" s="82"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="68"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="66"/>
+      <c r="A15" s="78"/>
       <c r="B15" s="4" t="s">
         <v>121</v>
       </c>
@@ -7556,7 +7556,7 @@
       <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="77"/>
+      <c r="A16" s="89"/>
       <c r="B16" s="18" t="s">
         <v>27</v>
       </c>
@@ -7569,18 +7569,18 @@
       <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="76">
+      <c r="A17" s="88">
         <v>5</v>
       </c>
-      <c r="B17" s="80" t="s">
+      <c r="B17" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
-      <c r="E17" s="82"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="68"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="66"/>
+      <c r="A18" s="78"/>
       <c r="B18" s="4" t="s">
         <v>122</v>
       </c>
@@ -7593,7 +7593,7 @@
       <c r="E18" s="17"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="77"/>
+      <c r="A19" s="89"/>
       <c r="B19" s="18" t="s">
         <v>21</v>
       </c>
@@ -7606,18 +7606,18 @@
       <c r="E19" s="16"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="73">
+      <c r="A20" s="85">
         <v>6</v>
       </c>
-      <c r="B20" s="86" t="s">
+      <c r="B20" s="74" t="s">
         <v>111</v>
       </c>
-      <c r="C20" s="87"/>
-      <c r="D20" s="87"/>
-      <c r="E20" s="88"/>
+      <c r="C20" s="75"/>
+      <c r="D20" s="75"/>
+      <c r="E20" s="76"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="74"/>
+      <c r="A21" s="86"/>
       <c r="B21" s="4" t="s">
         <v>123</v>
       </c>
@@ -7630,7 +7630,7 @@
       <c r="E21" s="33"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="74"/>
+      <c r="A22" s="86"/>
       <c r="B22" s="7" t="s">
         <v>112</v>
       </c>
@@ -7643,7 +7643,7 @@
       <c r="E22" s="28"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="75"/>
+      <c r="A23" s="87"/>
       <c r="B23" s="18" t="s">
         <v>113</v>
       </c>
@@ -7656,18 +7656,18 @@
       <c r="E23" s="36"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="76">
+      <c r="A24" s="88">
         <v>7</v>
       </c>
-      <c r="B24" s="86" t="s">
+      <c r="B24" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="88"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="76"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="66"/>
+      <c r="A25" s="78"/>
       <c r="B25" s="4" t="s">
         <v>137</v>
       </c>
@@ -7680,7 +7680,7 @@
       <c r="E25" s="33"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="77"/>
+      <c r="A26" s="89"/>
       <c r="B26" s="18" t="s">
         <v>116</v>
       </c>
@@ -7693,18 +7693,18 @@
       <c r="E26" s="36"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="76">
+      <c r="A27" s="88">
         <v>8</v>
       </c>
-      <c r="B27" s="89" t="s">
+      <c r="B27" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="88"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="76"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="66"/>
+      <c r="A28" s="78"/>
       <c r="B28" s="38" t="s">
         <v>136</v>
       </c>
@@ -7717,7 +7717,7 @@
       <c r="E28" s="33"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="77"/>
+      <c r="A29" s="89"/>
       <c r="B29" s="39" t="s">
         <v>138</v>
       </c>
@@ -7730,18 +7730,18 @@
       <c r="E29" s="31"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="76">
+      <c r="A30" s="88">
         <v>9</v>
       </c>
-      <c r="B30" s="89" t="s">
+      <c r="B30" s="77" t="s">
         <v>142</v>
       </c>
-      <c r="C30" s="87"/>
-      <c r="D30" s="87"/>
-      <c r="E30" s="88"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="76"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="66"/>
+      <c r="A31" s="78"/>
       <c r="B31" s="38" t="s">
         <v>143</v>
       </c>
@@ -7754,7 +7754,7 @@
       <c r="E31" s="33"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="77"/>
+      <c r="A32" s="89"/>
       <c r="B32" s="39" t="s">
         <v>144</v>
       </c>
@@ -7767,18 +7767,18 @@
       <c r="E32" s="31"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="70">
+      <c r="A33" s="82">
         <v>10</v>
       </c>
-      <c r="B33" s="80" t="s">
+      <c r="B33" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="81"/>
-      <c r="D33" s="81"/>
-      <c r="E33" s="82"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="68"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="71"/>
+      <c r="A34" s="83"/>
       <c r="B34" s="4" t="s">
         <v>132</v>
       </c>
@@ -7791,7 +7791,7 @@
       <c r="E34" s="21"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="71"/>
+      <c r="A35" s="83"/>
       <c r="B35" s="4" t="s">
         <v>117</v>
       </c>
@@ -7806,7 +7806,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="71"/>
+      <c r="A36" s="83"/>
       <c r="B36" s="7" t="s">
         <v>137</v>
       </c>
@@ -7821,7 +7821,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="71"/>
+      <c r="A37" s="83"/>
       <c r="B37" s="7" t="s">
         <v>136</v>
       </c>
@@ -7836,7 +7836,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="72"/>
+      <c r="A38" s="84"/>
       <c r="B38" s="18" t="s">
         <v>143</v>
       </c>
@@ -7847,22 +7847,22 @@
         <v>4</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="70">
+      <c r="A39" s="82">
         <v>11</v>
       </c>
-      <c r="B39" s="80" t="s">
+      <c r="B39" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="82"/>
+      <c r="C39" s="67"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="68"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="71"/>
+      <c r="A40" s="83"/>
       <c r="B40" s="4" t="s">
         <v>135</v>
       </c>
@@ -7875,7 +7875,7 @@
       <c r="E40" s="21"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="71"/>
+      <c r="A41" s="83"/>
       <c r="B41" s="4" t="s">
         <v>118</v>
       </c>
@@ -7890,7 +7890,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="71"/>
+      <c r="A42" s="83"/>
       <c r="B42" s="7" t="s">
         <v>137</v>
       </c>
@@ -7905,7 +7905,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="71"/>
+      <c r="A43" s="83"/>
       <c r="B43" s="7" t="s">
         <v>136</v>
       </c>
@@ -7920,7 +7920,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="72"/>
+      <c r="A44" s="84"/>
       <c r="B44" s="18" t="s">
         <v>143</v>
       </c>
@@ -7931,22 +7931,22 @@
         <v>29</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="70">
+      <c r="A45" s="82">
         <v>12</v>
       </c>
-      <c r="B45" s="80" t="s">
+      <c r="B45" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="81"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="82"/>
+      <c r="C45" s="67"/>
+      <c r="D45" s="67"/>
+      <c r="E45" s="68"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="71"/>
+      <c r="A46" s="83"/>
       <c r="B46" s="4" t="s">
         <v>124</v>
       </c>
@@ -7959,7 +7959,7 @@
       <c r="E46" s="17"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="71"/>
+      <c r="A47" s="83"/>
       <c r="B47" s="7" t="s">
         <v>120</v>
       </c>
@@ -7974,9 +7974,9 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="71"/>
+      <c r="A48" s="83"/>
       <c r="B48" s="7" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>7</v>
@@ -7985,13 +7985,13 @@
         <v>4</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="71"/>
+      <c r="A49" s="83"/>
       <c r="B49" s="4" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>7</v>
@@ -8000,11 +8000,11 @@
         <v>4</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="71"/>
+      <c r="A50" s="83"/>
       <c r="B50" s="7" t="s">
         <v>121</v>
       </c>
@@ -8015,11 +8015,11 @@
         <v>4</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="71"/>
+      <c r="A51" s="83"/>
       <c r="B51" s="7" t="s">
         <v>137</v>
       </c>
@@ -8034,7 +8034,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="71"/>
+      <c r="A52" s="83"/>
       <c r="B52" s="7" t="s">
         <v>136</v>
       </c>
@@ -8049,7 +8049,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="71"/>
+      <c r="A53" s="83"/>
       <c r="B53" s="7" t="s">
         <v>122</v>
       </c>
@@ -8064,7 +8064,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="72"/>
+      <c r="A54" s="84"/>
       <c r="B54" s="18" t="s">
         <v>20</v>
       </c>
@@ -8075,18 +8075,18 @@
       <c r="E54" s="16"/>
     </row>
     <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="70">
+      <c r="A55" s="82">
         <v>13</v>
       </c>
-      <c r="B55" s="80" t="s">
+      <c r="B55" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="81"/>
-      <c r="D55" s="81"/>
-      <c r="E55" s="82"/>
+      <c r="C55" s="67"/>
+      <c r="D55" s="67"/>
+      <c r="E55" s="68"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="71"/>
+      <c r="A56" s="83"/>
       <c r="B56" s="4" t="s">
         <v>128</v>
       </c>
@@ -8099,7 +8099,7 @@
       <c r="E56" s="21"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="71"/>
+      <c r="A57" s="83"/>
       <c r="B57" s="7" t="s">
         <v>124</v>
       </c>
@@ -8114,7 +8114,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="71"/>
+      <c r="A58" s="83"/>
       <c r="B58" s="7" t="s">
         <v>122</v>
       </c>
@@ -8129,7 +8129,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="72"/>
+      <c r="A59" s="84"/>
       <c r="B59" s="18" t="s">
         <v>19</v>
       </c>
@@ -8141,16 +8141,16 @@
     </row>
     <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="67"/>
-      <c r="B61" s="83" t="s">
+      <c r="A61" s="79"/>
+      <c r="B61" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="C61" s="84"/>
-      <c r="D61" s="84"/>
-      <c r="E61" s="85"/>
+      <c r="C61" s="72"/>
+      <c r="D61" s="72"/>
+      <c r="E61" s="73"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="68"/>
+      <c r="A62" s="80"/>
       <c r="B62" s="49" t="s">
         <v>119</v>
       </c>
@@ -8163,7 +8163,7 @@
       <c r="E62" s="52"/>
     </row>
     <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="69"/>
+      <c r="A63" s="81"/>
       <c r="B63" s="53" t="s">
         <v>26</v>
       </c>
@@ -8177,16 +8177,16 @@
     </row>
     <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="67"/>
-      <c r="B65" s="83" t="s">
+      <c r="A65" s="79"/>
+      <c r="B65" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="C65" s="84"/>
-      <c r="D65" s="84"/>
-      <c r="E65" s="85"/>
+      <c r="C65" s="72"/>
+      <c r="D65" s="72"/>
+      <c r="E65" s="73"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="68"/>
+      <c r="A66" s="80"/>
       <c r="B66" s="49" t="s">
         <v>130</v>
       </c>
@@ -8199,7 +8199,7 @@
       <c r="E66" s="57"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="68"/>
+      <c r="A67" s="80"/>
       <c r="B67" s="58" t="s">
         <v>117</v>
       </c>
@@ -8214,7 +8214,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="69"/>
+      <c r="A68" s="81"/>
       <c r="B68" s="53" t="s">
         <v>119</v>
       </c>
@@ -8230,16 +8230,16 @@
     </row>
     <row r="69" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="67"/>
-      <c r="B70" s="83" t="s">
+      <c r="A70" s="79"/>
+      <c r="B70" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="C70" s="84"/>
-      <c r="D70" s="84"/>
-      <c r="E70" s="85"/>
+      <c r="C70" s="72"/>
+      <c r="D70" s="72"/>
+      <c r="E70" s="73"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="68"/>
+      <c r="A71" s="80"/>
       <c r="B71" s="49" t="s">
         <v>133</v>
       </c>
@@ -8252,7 +8252,7 @@
       <c r="E71" s="57"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="68"/>
+      <c r="A72" s="80"/>
       <c r="B72" s="58" t="s">
         <v>118</v>
       </c>
@@ -8267,7 +8267,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="69"/>
+      <c r="A73" s="81"/>
       <c r="B73" s="53" t="s">
         <v>119</v>
       </c>
@@ -8283,6 +8283,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="A55:A59"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A45:A54"/>
+    <mergeCell ref="A39:A44"/>
     <mergeCell ref="B33:E33"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:E2"/>
@@ -8299,23 +8316,6 @@
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="A55:A59"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A45:A54"/>
-    <mergeCell ref="A39:A44"/>
-    <mergeCell ref="A33:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9019,7 +9019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99330B9-CAFA-4822-8F10-146FD06622F1}">
   <dimension ref="B1:AJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -9055,36 +9055,36 @@
   <sheetData>
     <row r="1" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="82"/>
-      <c r="F2" s="80" t="s">
+      <c r="C2" s="67"/>
+      <c r="D2" s="68"/>
+      <c r="F2" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="81"/>
-      <c r="H2" s="82"/>
-      <c r="J2" s="80" t="s">
+      <c r="G2" s="67"/>
+      <c r="H2" s="68"/>
+      <c r="J2" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="81"/>
-      <c r="L2" s="82"/>
-      <c r="N2" s="80" t="s">
+      <c r="K2" s="67"/>
+      <c r="L2" s="68"/>
+      <c r="N2" s="66" t="s">
         <v>141</v>
       </c>
-      <c r="O2" s="81"/>
-      <c r="P2" s="82"/>
-      <c r="R2" s="86" t="s">
+      <c r="O2" s="67"/>
+      <c r="P2" s="68"/>
+      <c r="R2" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="S2" s="87"/>
-      <c r="T2" s="88"/>
-      <c r="V2" s="86" t="s">
+      <c r="S2" s="75"/>
+      <c r="T2" s="76"/>
+      <c r="V2" s="74" t="s">
         <v>111</v>
       </c>
-      <c r="W2" s="87"/>
-      <c r="X2" s="88"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="76"/>
       <c r="AG2" s="45"/>
     </row>
     <row r="3" spans="2:36" x14ac:dyDescent="0.25">
@@ -9269,31 +9269,31 @@
     </row>
     <row r="9" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="81"/>
-      <c r="D10" s="82"/>
-      <c r="F10" s="80" t="s">
+      <c r="C10" s="67"/>
+      <c r="D10" s="68"/>
+      <c r="F10" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="81"/>
-      <c r="H10" s="82"/>
-      <c r="J10" s="80" t="s">
+      <c r="G10" s="67"/>
+      <c r="H10" s="68"/>
+      <c r="J10" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="81"/>
-      <c r="L10" s="82"/>
-      <c r="N10" s="80" t="s">
+      <c r="K10" s="67"/>
+      <c r="L10" s="68"/>
+      <c r="N10" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="O10" s="81"/>
-      <c r="P10" s="82"/>
-      <c r="R10" s="86" t="s">
+      <c r="O10" s="67"/>
+      <c r="P10" s="68"/>
+      <c r="R10" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="S10" s="87"/>
-      <c r="T10" s="88"/>
+      <c r="S10" s="75"/>
+      <c r="T10" s="76"/>
     </row>
     <row r="11" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
@@ -9561,11 +9561,11 @@
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
-      <c r="N20" s="80" t="s">
+      <c r="N20" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="O20" s="81"/>
-      <c r="P20" s="82"/>
+      <c r="O20" s="67"/>
+      <c r="P20" s="68"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N21" s="4" t="s">
@@ -9591,21 +9591,21 @@
     </row>
     <row r="32" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="83" t="s">
+      <c r="B33" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="84"/>
-      <c r="D33" s="85"/>
-      <c r="F33" s="83" t="s">
+      <c r="C33" s="72"/>
+      <c r="D33" s="73"/>
+      <c r="F33" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="G33" s="84"/>
-      <c r="H33" s="85"/>
-      <c r="J33" s="83" t="s">
+      <c r="G33" s="72"/>
+      <c r="H33" s="73"/>
+      <c r="J33" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="K33" s="84"/>
-      <c r="L33" s="85"/>
+      <c r="K33" s="72"/>
+      <c r="L33" s="73"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="49" t="s">
@@ -9687,13 +9687,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="J2:L2"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="F33:H33"/>
     <mergeCell ref="N10:P10"/>
@@ -9703,6 +9696,13 @@
     <mergeCell ref="N20:P20"/>
     <mergeCell ref="J33:L33"/>
     <mergeCell ref="B17:D17"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="J2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
tables are good and populated
</commit_message>
<xml_diff>
--- a/Tables&Relations.xlsx
+++ b/Tables&Relations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgrifit\Desktop\IIT\OnlineTraining\Spring2018\OpenSourceProgramming\FinalProject_DueApr29\ghrepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E4C01D-6FC7-4026-AF2B-CD5021068236}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F1921D-BFE9-4A47-A48D-81101946E202}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20355" windowHeight="10830" xr2:uid="{F62A5D56-28AC-4B05-9321-33328E52EE30}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20355" windowHeight="10830" firstSheet="1" activeTab="1" xr2:uid="{F62A5D56-28AC-4B05-9321-33328E52EE30}"/>
   </bookViews>
   <sheets>
     <sheet name="Table Relations" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="176">
   <si>
     <t>fname</t>
   </si>
@@ -149,9 +149,6 @@
     <t>Brett</t>
   </si>
   <si>
-    <t>Malcom</t>
-  </si>
-  <si>
     <t>Winston</t>
   </si>
   <si>
@@ -552,6 +549,12 @@
   </si>
   <si>
     <t>Reference Nurse Availability - nurse_id</t>
+  </si>
+  <si>
+    <t>Malcolm</t>
+  </si>
+  <si>
+    <t>start_time_id</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1068,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1214,6 +1217,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1222,6 +1235,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1249,42 +1289,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -7355,7 +7359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D224C6BA-3041-4FF2-9ED2-49CADB590F58}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="B21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
@@ -7372,30 +7376,30 @@
       <c r="A1" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="69"/>
-      <c r="D1" s="70"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="83"/>
       <c r="E1" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="78">
+      <c r="A2" s="73">
         <v>1</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="68"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="72"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="78"/>
+      <c r="A3" s="73"/>
       <c r="B3" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>7</v>
@@ -7406,7 +7410,7 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="78"/>
+      <c r="A4" s="73"/>
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
@@ -7419,7 +7423,7 @@
       <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="78"/>
+      <c r="A5" s="73"/>
       <c r="B5" s="10" t="s">
         <v>1</v>
       </c>
@@ -7432,20 +7436,20 @@
       <c r="E5" s="15"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="88">
+      <c r="A6" s="80">
         <v>2</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="68"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="72"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="78"/>
+      <c r="A7" s="73"/>
       <c r="B7" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>7</v>
@@ -7456,7 +7460,7 @@
       <c r="E7" s="17"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="78"/>
+      <c r="A8" s="73"/>
       <c r="B8" s="7" t="s">
         <v>0</v>
       </c>
@@ -7469,7 +7473,7 @@
       <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="89"/>
+      <c r="A9" s="81"/>
       <c r="B9" s="18" t="s">
         <v>0</v>
       </c>
@@ -7482,20 +7486,20 @@
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="88">
+      <c r="A10" s="80">
         <v>3</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="68"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="72"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="78"/>
+      <c r="A11" s="73"/>
       <c r="B11" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>7</v>
@@ -7506,7 +7510,7 @@
       <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="78"/>
+      <c r="A12" s="73"/>
       <c r="B12" s="7" t="s">
         <v>0</v>
       </c>
@@ -7519,7 +7523,7 @@
       <c r="E12" s="14"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="89"/>
+      <c r="A13" s="81"/>
       <c r="B13" s="18" t="s">
         <v>1</v>
       </c>
@@ -7532,20 +7536,20 @@
       <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="88">
+      <c r="A14" s="80">
         <v>4</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="68"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="72"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="78"/>
+      <c r="A15" s="73"/>
       <c r="B15" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>7</v>
@@ -7556,7 +7560,7 @@
       <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="89"/>
+      <c r="A16" s="81"/>
       <c r="B16" s="18" t="s">
         <v>27</v>
       </c>
@@ -7569,20 +7573,20 @@
       <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="88">
+      <c r="A17" s="80">
         <v>5</v>
       </c>
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="68"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="72"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="78"/>
+      <c r="A18" s="73"/>
       <c r="B18" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>7</v>
@@ -7593,7 +7597,7 @@
       <c r="E18" s="17"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="89"/>
+      <c r="A19" s="81"/>
       <c r="B19" s="18" t="s">
         <v>21</v>
       </c>
@@ -7606,20 +7610,20 @@
       <c r="E19" s="16"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="85">
+      <c r="A20" s="77">
         <v>6</v>
       </c>
-      <c r="B20" s="74" t="s">
-        <v>111</v>
-      </c>
-      <c r="C20" s="75"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="76"/>
+      <c r="B20" s="87" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="88"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="89"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="86"/>
+      <c r="A21" s="78"/>
       <c r="B21" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>7</v>
@@ -7630,9 +7634,9 @@
       <c r="E21" s="33"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="86"/>
+      <c r="A22" s="78"/>
       <c r="B22" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>8</v>
@@ -7643,9 +7647,9 @@
       <c r="E22" s="28"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="87"/>
+      <c r="A23" s="79"/>
       <c r="B23" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C23" s="34" t="s">
         <v>8</v>
@@ -7656,20 +7660,20 @@
       <c r="E23" s="36"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="88">
+      <c r="A24" s="80">
         <v>7</v>
       </c>
-      <c r="B24" s="74" t="s">
-        <v>114</v>
-      </c>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="76"/>
+      <c r="B24" s="87" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="89"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="78"/>
+      <c r="A25" s="73"/>
       <c r="B25" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C25" s="37" t="s">
         <v>7</v>
@@ -7680,9 +7684,9 @@
       <c r="E25" s="33"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="89"/>
+      <c r="A26" s="81"/>
       <c r="B26" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C26" s="34" t="s">
         <v>8</v>
@@ -7693,20 +7697,20 @@
       <c r="E26" s="36"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="88">
+      <c r="A27" s="80">
         <v>8</v>
       </c>
-      <c r="B27" s="77" t="s">
-        <v>115</v>
-      </c>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="76"/>
+      <c r="B27" s="90" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="88"/>
+      <c r="D27" s="88"/>
+      <c r="E27" s="89"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="78"/>
+      <c r="A28" s="73"/>
       <c r="B28" s="38" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C28" s="37" t="s">
         <v>7</v>
@@ -7717,9 +7721,9 @@
       <c r="E28" s="33"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="89"/>
+      <c r="A29" s="81"/>
       <c r="B29" s="39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C29" s="29" t="s">
         <v>8</v>
@@ -7730,20 +7734,20 @@
       <c r="E29" s="31"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="88">
+      <c r="A30" s="80">
         <v>9</v>
       </c>
-      <c r="B30" s="77" t="s">
+      <c r="B30" s="90" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" s="88"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="89"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="73"/>
+      <c r="B31" s="38" t="s">
         <v>142</v>
-      </c>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="76"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="78"/>
-      <c r="B31" s="38" t="s">
-        <v>143</v>
       </c>
       <c r="C31" s="37" t="s">
         <v>7</v>
@@ -7754,9 +7758,9 @@
       <c r="E31" s="33"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="89"/>
+      <c r="A32" s="81"/>
       <c r="B32" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C32" s="29" t="s">
         <v>8</v>
@@ -7767,20 +7771,20 @@
       <c r="E32" s="31"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="82">
+      <c r="A33" s="67">
         <v>10</v>
       </c>
-      <c r="B33" s="66" t="s">
+      <c r="B33" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="68"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="72"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="83"/>
+      <c r="A34" s="68"/>
       <c r="B34" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>7</v>
@@ -7791,9 +7795,9 @@
       <c r="E34" s="21"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="83"/>
+      <c r="A35" s="68"/>
       <c r="B35" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>7</v>
@@ -7802,13 +7806,13 @@
         <v>4</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="83"/>
+      <c r="A36" s="68"/>
       <c r="B36" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>8</v>
@@ -7817,13 +7821,13 @@
         <v>4</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="83"/>
+      <c r="A37" s="68"/>
       <c r="B37" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>8</v>
@@ -7832,13 +7836,13 @@
         <v>4</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="84"/>
+      <c r="A38" s="69"/>
       <c r="B38" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C38" s="19" t="s">
         <v>10</v>
@@ -7847,24 +7851,24 @@
         <v>4</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="82">
+      <c r="A39" s="67">
         <v>11</v>
       </c>
-      <c r="B39" s="66" t="s">
+      <c r="B39" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="67"/>
-      <c r="D39" s="67"/>
-      <c r="E39" s="68"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="72"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="83"/>
+      <c r="A40" s="68"/>
       <c r="B40" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>7</v>
@@ -7875,9 +7879,9 @@
       <c r="E40" s="21"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="83"/>
+      <c r="A41" s="68"/>
       <c r="B41" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>7</v>
@@ -7886,13 +7890,13 @@
         <v>4</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="83"/>
+      <c r="A42" s="68"/>
       <c r="B42" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>8</v>
@@ -7901,13 +7905,13 @@
         <v>29</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="83"/>
+      <c r="A43" s="68"/>
       <c r="B43" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>9</v>
@@ -7916,13 +7920,13 @@
         <v>29</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="84"/>
+      <c r="A44" s="69"/>
       <c r="B44" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>10</v>
@@ -7931,24 +7935,24 @@
         <v>29</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="82">
+      <c r="A45" s="67">
         <v>12</v>
       </c>
-      <c r="B45" s="66" t="s">
+      <c r="B45" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="67"/>
-      <c r="D45" s="67"/>
-      <c r="E45" s="68"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="72"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="83"/>
+      <c r="A46" s="68"/>
       <c r="B46" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>7</v>
@@ -7959,9 +7963,9 @@
       <c r="E46" s="17"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="83"/>
+      <c r="A47" s="68"/>
       <c r="B47" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>7</v>
@@ -7970,13 +7974,13 @@
         <v>4</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="83"/>
+      <c r="A48" s="68"/>
       <c r="B48" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>7</v>
@@ -7985,13 +7989,13 @@
         <v>4</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="83"/>
+      <c r="A49" s="68"/>
       <c r="B49" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>7</v>
@@ -8000,13 +8004,13 @@
         <v>4</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="83"/>
+      <c r="A50" s="68"/>
       <c r="B50" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>7</v>
@@ -8015,13 +8019,13 @@
         <v>4</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="83"/>
+      <c r="A51" s="68"/>
       <c r="B51" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>8</v>
@@ -8030,13 +8034,13 @@
         <v>30</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="83"/>
+      <c r="A52" s="68"/>
       <c r="B52" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>8</v>
@@ -8045,13 +8049,13 @@
         <v>30</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="83"/>
+      <c r="A53" s="68"/>
       <c r="B53" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>7</v>
@@ -8060,11 +8064,11 @@
         <v>4</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="84"/>
+      <c r="A54" s="69"/>
       <c r="B54" s="18" t="s">
         <v>20</v>
       </c>
@@ -8075,20 +8079,20 @@
       <c r="E54" s="16"/>
     </row>
     <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="82">
+      <c r="A55" s="67">
         <v>13</v>
       </c>
-      <c r="B55" s="66" t="s">
+      <c r="B55" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="67"/>
-      <c r="D55" s="67"/>
-      <c r="E55" s="68"/>
+      <c r="C55" s="71"/>
+      <c r="D55" s="71"/>
+      <c r="E55" s="72"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="83"/>
+      <c r="A56" s="68"/>
       <c r="B56" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>7</v>
@@ -8099,9 +8103,9 @@
       <c r="E56" s="21"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="83"/>
+      <c r="A57" s="68"/>
       <c r="B57" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>7</v>
@@ -8110,13 +8114,13 @@
         <v>4</v>
       </c>
       <c r="E57" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="83"/>
+      <c r="A58" s="68"/>
       <c r="B58" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>7</v>
@@ -8125,11 +8129,11 @@
         <v>29</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="84"/>
+      <c r="A59" s="69"/>
       <c r="B59" s="18" t="s">
         <v>19</v>
       </c>
@@ -8141,18 +8145,18 @@
     </row>
     <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="79"/>
-      <c r="B61" s="71" t="s">
+      <c r="A61" s="74"/>
+      <c r="B61" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="C61" s="72"/>
-      <c r="D61" s="72"/>
-      <c r="E61" s="73"/>
+      <c r="C61" s="85"/>
+      <c r="D61" s="85"/>
+      <c r="E61" s="86"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="80"/>
+      <c r="A62" s="75"/>
       <c r="B62" s="49" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C62" s="50" t="s">
         <v>7</v>
@@ -8163,7 +8167,7 @@
       <c r="E62" s="52"/>
     </row>
     <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="81"/>
+      <c r="A63" s="76"/>
       <c r="B63" s="53" t="s">
         <v>26</v>
       </c>
@@ -8177,18 +8181,18 @@
     </row>
     <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="79"/>
-      <c r="B65" s="71" t="s">
+      <c r="A65" s="74"/>
+      <c r="B65" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="C65" s="72"/>
-      <c r="D65" s="72"/>
-      <c r="E65" s="73"/>
+      <c r="C65" s="85"/>
+      <c r="D65" s="85"/>
+      <c r="E65" s="86"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="80"/>
+      <c r="A66" s="75"/>
       <c r="B66" s="49" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C66" s="50" t="s">
         <v>7</v>
@@ -8199,9 +8203,9 @@
       <c r="E66" s="57"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="80"/>
+      <c r="A67" s="75"/>
       <c r="B67" s="58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C67" s="59" t="s">
         <v>7</v>
@@ -8210,13 +8214,13 @@
         <v>29</v>
       </c>
       <c r="E67" s="61" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="81"/>
+      <c r="A68" s="76"/>
       <c r="B68" s="53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C68" s="54" t="s">
         <v>7</v>
@@ -8225,23 +8229,23 @@
         <v>4</v>
       </c>
       <c r="E68" s="62" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="79"/>
-      <c r="B70" s="71" t="s">
+      <c r="A70" s="74"/>
+      <c r="B70" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="C70" s="72"/>
-      <c r="D70" s="72"/>
-      <c r="E70" s="73"/>
+      <c r="C70" s="85"/>
+      <c r="D70" s="85"/>
+      <c r="E70" s="86"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="80"/>
+      <c r="A71" s="75"/>
       <c r="B71" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C71" s="50" t="s">
         <v>7</v>
@@ -8252,9 +8256,9 @@
       <c r="E71" s="57"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="80"/>
+      <c r="A72" s="75"/>
       <c r="B72" s="58" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C72" s="59" t="s">
         <v>7</v>
@@ -8263,13 +8267,13 @@
         <v>29</v>
       </c>
       <c r="E72" s="61" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="81"/>
+      <c r="A73" s="76"/>
       <c r="B73" s="53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C73" s="54" t="s">
         <v>7</v>
@@ -8278,11 +8282,28 @@
         <v>29</v>
       </c>
       <c r="E73" s="62" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B10:E10"/>
     <mergeCell ref="A33:A38"/>
     <mergeCell ref="B39:E39"/>
     <mergeCell ref="A2:A5"/>
@@ -8299,23 +8320,6 @@
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A45:A54"/>
-    <mergeCell ref="A39:A44"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B30:E30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8326,8 +8330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035F8F-4CA6-41CD-B35D-614D8FDC778B}">
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8342,19 +8346,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="G1" s="90" t="s">
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="G1" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="90"/>
-      <c r="L1" s="90" t="s">
-        <v>150</v>
-      </c>
-      <c r="M1" s="90"/>
+      <c r="H1" s="91"/>
+      <c r="L1" s="91" t="s">
+        <v>149</v>
+      </c>
+      <c r="M1" s="91"/>
       <c r="S1" s="2" t="s">
         <v>23</v>
       </c>
@@ -8362,7 +8366,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -8371,16 +8375,16 @@
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="L2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>34</v>
@@ -8403,19 +8407,19 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L3" s="1">
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="S3" s="1">
         <v>1</v>
       </c>
       <c r="T3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -8432,19 +8436,19 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L4" s="1">
         <v>2</v>
       </c>
       <c r="M4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S4" s="1">
         <v>2</v>
       </c>
       <c r="T4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -8455,25 +8459,25 @@
         <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>174</v>
       </c>
       <c r="G5" s="1">
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L5" s="1">
         <v>3</v>
       </c>
       <c r="M5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S5" s="1">
         <v>3</v>
       </c>
       <c r="T5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -8481,28 +8485,28 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
         <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>42</v>
       </c>
       <c r="G6" s="1">
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L6" s="1">
         <v>4</v>
       </c>
       <c r="M6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="S6" s="1">
         <v>4</v>
       </c>
       <c r="T6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -8510,28 +8514,28 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
         <v>43</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
       </c>
       <c r="G7" s="1">
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L7" s="1">
         <v>5</v>
       </c>
       <c r="M7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S7" s="1">
         <v>5</v>
       </c>
       <c r="T7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -8539,23 +8543,23 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
         <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
       </c>
       <c r="G8" s="1">
         <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L8" s="1"/>
       <c r="S8" s="1">
         <v>6</v>
       </c>
       <c r="T8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -8563,16 +8567,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
         <v>47</v>
-      </c>
-      <c r="C9" t="s">
-        <v>48</v>
       </c>
       <c r="G9" s="1">
         <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L9" s="1"/>
     </row>
@@ -8581,16 +8585,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
         <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
       </c>
       <c r="G10" s="1">
         <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L10" s="1"/>
     </row>
@@ -8599,38 +8603,38 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
         <v>51</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
       </c>
       <c r="G11" s="1">
         <v>9</v>
       </c>
       <c r="H11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:20" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="90" t="s">
+      <c r="A13" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="90"/>
-      <c r="C13" s="90"/>
-      <c r="G13" s="90" t="s">
-        <v>102</v>
-      </c>
-      <c r="H13" s="90"/>
-      <c r="L13" s="90" t="s">
-        <v>142</v>
-      </c>
-      <c r="M13" s="90"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="91"/>
+      <c r="G13" s="91" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" s="91"/>
+      <c r="L13" s="91" t="s">
+        <v>141</v>
+      </c>
+      <c r="M13" s="91"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -8639,16 +8643,16 @@
         <v>1</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="L14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -8656,22 +8660,22 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
         <v>53</v>
-      </c>
-      <c r="C15" t="s">
-        <v>54</v>
       </c>
       <c r="G15" s="1">
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L15" s="1">
         <v>1</v>
       </c>
       <c r="M15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -8679,22 +8683,22 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G16" s="1">
         <v>2</v>
       </c>
       <c r="H16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L16" s="1">
         <v>2</v>
       </c>
       <c r="M16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -8702,16 +8706,16 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
         <v>56</v>
-      </c>
-      <c r="C17" t="s">
-        <v>57</v>
       </c>
       <c r="G17" s="1">
         <v>3</v>
       </c>
       <c r="H17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -8719,27 +8723,27 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
         <v>58</v>
-      </c>
-      <c r="C18" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="90" t="s">
+      <c r="A20" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="90"/>
-      <c r="C20" s="90"/>
-      <c r="G20" s="90" t="s">
-        <v>157</v>
-      </c>
-      <c r="H20" s="90"/>
+      <c r="B20" s="91"/>
+      <c r="C20" s="91"/>
+      <c r="G20" s="91" t="s">
+        <v>156</v>
+      </c>
+      <c r="H20" s="91"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>0</v>
@@ -8747,11 +8751,11 @@
       <c r="C21" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="1">
-        <v>1</v>
-      </c>
-      <c r="H21" t="s">
-        <v>158</v>
+      <c r="G21" s="66" t="s">
+        <v>175</v>
+      </c>
+      <c r="H21" s="66" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -8759,16 +8763,16 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" t="s">
         <v>60</v>
       </c>
-      <c r="C22" t="s">
-        <v>61</v>
-      </c>
       <c r="G22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -8776,16 +8780,16 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
         <v>62</v>
       </c>
-      <c r="C23" t="s">
-        <v>63</v>
-      </c>
       <c r="G23" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H23" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -8793,16 +8797,16 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" t="s">
         <v>64</v>
       </c>
-      <c r="C24" t="s">
-        <v>65</v>
-      </c>
       <c r="G24" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -8810,16 +8814,16 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" t="s">
         <v>66</v>
       </c>
-      <c r="C25" t="s">
-        <v>67</v>
-      </c>
       <c r="G25" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H25" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -8827,16 +8831,16 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" t="s">
         <v>68</v>
       </c>
-      <c r="C26" t="s">
-        <v>69</v>
-      </c>
       <c r="G26" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -8844,16 +8848,16 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" t="s">
         <v>70</v>
       </c>
-      <c r="C27" t="s">
-        <v>71</v>
-      </c>
       <c r="G27" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H27" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -8861,16 +8865,16 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" t="s">
         <v>72</v>
       </c>
-      <c r="C28" t="s">
-        <v>73</v>
-      </c>
       <c r="G28" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -8878,16 +8882,16 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" t="s">
         <v>74</v>
       </c>
-      <c r="C29" t="s">
-        <v>75</v>
-      </c>
       <c r="G29" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H29" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -8895,10 +8899,16 @@
         <v>9</v>
       </c>
       <c r="B30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" t="s">
         <v>76</v>
       </c>
-      <c r="C30" t="s">
-        <v>77</v>
+      <c r="G30" s="1">
+        <v>9</v>
+      </c>
+      <c r="H30" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -8906,10 +8916,10 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" t="s">
         <v>78</v>
-      </c>
-      <c r="C31" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -8917,10 +8927,10 @@
         <v>11</v>
       </c>
       <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" t="s">
         <v>80</v>
-      </c>
-      <c r="C32" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -8928,10 +8938,10 @@
         <v>12</v>
       </c>
       <c r="B33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" t="s">
         <v>82</v>
-      </c>
-      <c r="C33" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -8939,10 +8949,10 @@
         <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -8950,10 +8960,10 @@
         <v>14</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -8961,10 +8971,10 @@
         <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -8972,10 +8982,10 @@
         <v>16</v>
       </c>
       <c r="B37" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" t="s">
         <v>87</v>
-      </c>
-      <c r="C37" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -8983,10 +8993,10 @@
         <v>17</v>
       </c>
       <c r="B38" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" t="s">
         <v>89</v>
-      </c>
-      <c r="C38" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -8994,10 +9004,10 @@
         <v>18</v>
       </c>
       <c r="B39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" t="s">
         <v>91</v>
-      </c>
-      <c r="C39" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -9055,41 +9065,41 @@
   <sheetData>
     <row r="1" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="68"/>
-      <c r="F2" s="66" t="s">
+      <c r="C2" s="71"/>
+      <c r="D2" s="72"/>
+      <c r="F2" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68"/>
-      <c r="J2" s="66" t="s">
+      <c r="G2" s="71"/>
+      <c r="H2" s="72"/>
+      <c r="J2" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="67"/>
-      <c r="L2" s="68"/>
-      <c r="N2" s="66" t="s">
-        <v>141</v>
-      </c>
-      <c r="O2" s="67"/>
-      <c r="P2" s="68"/>
-      <c r="R2" s="74" t="s">
-        <v>114</v>
-      </c>
-      <c r="S2" s="75"/>
-      <c r="T2" s="76"/>
-      <c r="V2" s="74" t="s">
-        <v>111</v>
-      </c>
-      <c r="W2" s="75"/>
-      <c r="X2" s="76"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="72"/>
+      <c r="N2" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="O2" s="71"/>
+      <c r="P2" s="72"/>
+      <c r="R2" s="87" t="s">
+        <v>113</v>
+      </c>
+      <c r="S2" s="88"/>
+      <c r="T2" s="89"/>
+      <c r="V2" s="87" t="s">
+        <v>110</v>
+      </c>
+      <c r="W2" s="88"/>
+      <c r="X2" s="89"/>
       <c r="AG2" s="45"/>
     </row>
     <row r="3" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>7</v>
@@ -9098,7 +9108,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>7</v>
@@ -9107,7 +9117,7 @@
         <v>3</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>7</v>
@@ -9116,7 +9126,7 @@
         <v>3</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>7</v>
@@ -9125,7 +9135,7 @@
         <v>3</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="S3" s="37" t="s">
         <v>7</v>
@@ -9134,7 +9144,7 @@
         <v>3</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="W3" s="5" t="s">
         <v>7</v>
@@ -9182,7 +9192,7 @@
         <v>10</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S4" s="29" t="s">
         <v>8</v>
@@ -9191,7 +9201,7 @@
         <v>8</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="W4" s="8" t="s">
         <v>8</v>
@@ -9230,7 +9240,7 @@
         <v>30</v>
       </c>
       <c r="V5" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W5" s="29" t="s">
         <v>8</v>
@@ -9269,35 +9279,35 @@
     </row>
     <row r="9" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="67"/>
-      <c r="D10" s="68"/>
-      <c r="F10" s="66" t="s">
+      <c r="C10" s="71"/>
+      <c r="D10" s="72"/>
+      <c r="F10" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="67"/>
-      <c r="H10" s="68"/>
-      <c r="J10" s="66" t="s">
+      <c r="G10" s="71"/>
+      <c r="H10" s="72"/>
+      <c r="J10" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="67"/>
-      <c r="L10" s="68"/>
-      <c r="N10" s="66" t="s">
+      <c r="K10" s="71"/>
+      <c r="L10" s="72"/>
+      <c r="N10" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="O10" s="67"/>
-      <c r="P10" s="68"/>
-      <c r="R10" s="74" t="s">
-        <v>115</v>
-      </c>
-      <c r="S10" s="75"/>
-      <c r="T10" s="76"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="72"/>
+      <c r="R10" s="87" t="s">
+        <v>114</v>
+      </c>
+      <c r="S10" s="88"/>
+      <c r="T10" s="89"/>
     </row>
     <row r="11" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>7</v>
@@ -9306,7 +9316,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>7</v>
@@ -9315,7 +9325,7 @@
         <v>3</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>7</v>
@@ -9324,7 +9334,7 @@
         <v>3</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O11" s="5" t="s">
         <v>7</v>
@@ -9333,7 +9343,7 @@
         <v>3</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="S11" s="37" t="s">
         <v>7</v>
@@ -9344,7 +9354,7 @@
     </row>
     <row r="12" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>7</v>
@@ -9353,7 +9363,7 @@
         <v>4</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>7</v>
@@ -9362,7 +9372,7 @@
         <v>4</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>7</v>
@@ -9371,7 +9381,7 @@
         <v>4</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O12" s="8" t="s">
         <v>7</v>
@@ -9380,7 +9390,7 @@
         <v>4</v>
       </c>
       <c r="R12" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S12" s="29" t="s">
         <v>8</v>
@@ -9391,7 +9401,7 @@
     </row>
     <row r="13" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>8</v>
@@ -9400,7 +9410,7 @@
         <v>4</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>8</v>
@@ -9409,7 +9419,7 @@
         <v>29</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>7</v>
@@ -9418,7 +9428,7 @@
         <v>4</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O13" s="8" t="s">
         <v>7</v>
@@ -9447,7 +9457,7 @@
         <v>29</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K14" s="8" t="s">
         <v>7</v>
@@ -9465,7 +9475,7 @@
     </row>
     <row r="15" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>10</v>
@@ -9474,7 +9484,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>10</v>
@@ -9483,7 +9493,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>7</v>
@@ -9494,7 +9504,7 @@
     </row>
     <row r="16" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J16" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>8</v>
@@ -9504,13 +9514,13 @@
       </c>
     </row>
     <row r="17" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="91" t="s">
-        <v>142</v>
-      </c>
-      <c r="C17" s="92"/>
-      <c r="D17" s="93"/>
+      <c r="B17" s="92" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" s="93"/>
+      <c r="D17" s="94"/>
       <c r="J17" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>8</v>
@@ -9521,7 +9531,7 @@
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C18" s="48" t="s">
         <v>7</v>
@@ -9530,7 +9540,7 @@
         <v>3</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K18" s="8" t="s">
         <v>7</v>
@@ -9541,7 +9551,7 @@
     </row>
     <row r="19" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C19" s="29" t="s">
         <v>8</v>
@@ -9561,15 +9571,15 @@
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
-      <c r="N20" s="66" t="s">
+      <c r="N20" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="O20" s="67"/>
-      <c r="P20" s="68"/>
+      <c r="O20" s="71"/>
+      <c r="P20" s="72"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N21" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O21" s="5" t="s">
         <v>7</v>
@@ -9591,25 +9601,25 @@
     </row>
     <row r="32" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="71" t="s">
+      <c r="B33" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="72"/>
-      <c r="D33" s="73"/>
-      <c r="F33" s="71" t="s">
+      <c r="C33" s="85"/>
+      <c r="D33" s="86"/>
+      <c r="F33" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="G33" s="72"/>
-      <c r="H33" s="73"/>
-      <c r="J33" s="71" t="s">
+      <c r="G33" s="85"/>
+      <c r="H33" s="86"/>
+      <c r="J33" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="K33" s="72"/>
-      <c r="L33" s="73"/>
+      <c r="K33" s="85"/>
+      <c r="L33" s="86"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="49" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C34" s="50" t="s">
         <v>7</v>
@@ -9618,7 +9628,7 @@
         <v>3</v>
       </c>
       <c r="F34" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G34" s="50" t="s">
         <v>7</v>
@@ -9627,7 +9637,7 @@
         <v>3</v>
       </c>
       <c r="J34" s="49" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K34" s="50" t="s">
         <v>7</v>
@@ -9638,7 +9648,7 @@
     </row>
     <row r="35" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C35" s="59" t="s">
         <v>7</v>
@@ -9647,7 +9657,7 @@
         <v>29</v>
       </c>
       <c r="F35" s="58" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G35" s="59" t="s">
         <v>7</v>
@@ -9667,7 +9677,7 @@
     </row>
     <row r="36" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="63" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C36" s="64" t="s">
         <v>7</v>
@@ -9676,7 +9686,7 @@
         <v>4</v>
       </c>
       <c r="F36" s="63" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G36" s="64" t="s">
         <v>7</v>
@@ -9687,6 +9697,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="J2:L2"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="F33:H33"/>
     <mergeCell ref="N10:P10"/>
@@ -9696,13 +9713,6 @@
     <mergeCell ref="N20:P20"/>
     <mergeCell ref="J33:L33"/>
     <mergeCell ref="B17:D17"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="J2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>